<commit_message>
reference parameter completed! bug fixed when calculating address of local variable and outer variable
</commit_message>
<xml_diff>
--- a/DesignDocs/D1 符号表设计.xlsx
+++ b/DesignDocs/D1 符号表设计.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
   <si>
     <t>符号表设计</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -110,14 +110,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>useCount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>引用的次数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>addr</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -219,18 +211,6 @@
   </si>
   <si>
     <t>对不符合语义结构的单词，进行错误局部化处理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>对应四元式的标号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>quaternaryAddress</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -238,7 +218,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,9 +235,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -287,13 +273,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -595,13 +582,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
@@ -614,22 +601,22 @@
     <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -640,25 +627,25 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
         <v>33</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>34</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>35</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>36</v>
       </c>
-      <c r="H2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -669,25 +656,25 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -698,83 +685,83 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -782,28 +769,28 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -814,25 +801,25 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -843,25 +830,25 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -872,124 +859,85 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3">
       <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3">
       <c r="A22">
-        <v>3</v>
-      </c>
-      <c r="B22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A23">
-        <v>4</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A24">
-        <v>5</v>
-      </c>
-      <c r="B24" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1009,7 +957,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1022,7 +970,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>